<commit_message>
Data for question 4.29.
</commit_message>
<xml_diff>
--- a/data/Table1.5.xlsx
+++ b/data/Table1.5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Applied-Multivariate-Statistical-Analysis-Solutions\Applied-Multivariate-Statistical-Analysis-Solutions\Applied-Multivariate-Statistical-Analysis-Solutions\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1F382F-7D9B-46F4-8589-9F71D0E2C055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF23D76A-20D9-4EF0-82E9-56EC8A7BF67B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAC1AC7B-8047-4A3B-AA9F-1D9F4A9D0FAD}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,6 +180,13 @@
       <color theme="0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -524,8 +531,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -903,35 +911,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D55B92-36F2-4BE4-B96A-5C90406BF65B}">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="3.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="15">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>